<commit_message>
projeto quase finalizado, faltando site de suporte
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d42371d61bd3278c/Área de Trabalho/Atividades EAD/ADS/Pesquisa e Inovação/Projeto Individual/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d42371d61bd3278c/Área de Trabalho/Projeto Individual/RaidOracles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A9E7626-A170-404E-95CD-79C13FF36209}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{1A9E7626-A170-404E-95CD-79C13FF36209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89174705-F013-41BC-9E31-740E821BBD6F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0E7FD534-9141-4A92-9C54-60D89780E819}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Requisitos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Tarefa</t>
   </si>
@@ -51,18 +52,9 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Em andamento</t>
-  </si>
-  <si>
-    <t>Pendente</t>
-  </si>
-  <si>
     <t>Prioridade</t>
   </si>
   <si>
-    <t>Previsão</t>
-  </si>
-  <si>
     <t>Desenvolvimento do site</t>
   </si>
   <si>
@@ -79,6 +71,57 @@
   </si>
   <si>
     <t>Média</t>
+  </si>
+  <si>
+    <t>Concluído</t>
+  </si>
+  <si>
+    <t>Modelo lógico</t>
+  </si>
+  <si>
+    <t>Ferramenta de suporte</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>Requisitos</t>
+  </si>
+  <si>
+    <t>Classificação</t>
+  </si>
+  <si>
+    <t>Tamanho</t>
+  </si>
+  <si>
+    <t>Ordem Execução</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Site institucional</t>
+  </si>
+  <si>
+    <t>Essencial</t>
+  </si>
+  <si>
+    <t>Banco de dados</t>
+  </si>
+  <si>
+    <t>Conexão pela API Projeto Site</t>
+  </si>
+  <si>
+    <t>Gráfico informativo</t>
+  </si>
+  <si>
+    <t>Desejável</t>
+  </si>
+  <si>
+    <t>Página de publicações</t>
+  </si>
+  <si>
+    <t>Importante</t>
   </si>
 </sst>
 </file>
@@ -146,17 +189,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{45B0D38E-80B8-4742-AA00-221A5903E47C}" name="Tabela1" displayName="Tabela1" ref="A1:G5" totalsRowShown="0">
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{45B0D38E-80B8-4742-AA00-221A5903E47C}" name="Tabela1" displayName="Tabela1" ref="A1:F7" totalsRowShown="0">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{3AEDC75F-0C46-4CC2-8057-F874C9909F95}" name="Tarefa"/>
     <tableColumn id="2" xr3:uid="{AA2CEF05-8CA8-4356-BA2C-D87A87FF6CFD}" name="Início" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{8D981F89-EBF7-482A-9696-5FF28E725A5C}" name="Término" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{1D068AA5-9DDC-46B7-998B-EB7C65E8A5EB}" name="Duração (dias)" dataDxfId="0">
-      <calculatedColumnFormula>IF(Tabela1[[#This Row],[Término]]=0, "Não finalizado",(Tabela1[[#This Row],[Início]]-Tabela1[[#This Row],[Término]]))</calculatedColumnFormula>
+      <calculatedColumnFormula>Tabela1[[#This Row],[Término]]-Tabela1[[#This Row],[Início]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{A3FC0B33-96E6-4FB7-A2DE-391CE5257B1F}" name="Status"/>
     <tableColumn id="6" xr3:uid="{A8B61C61-60E4-48F0-9C21-C62D00D81032}" name="Prioridade"/>
-    <tableColumn id="7" xr3:uid="{2ACB2F32-3A91-4315-989A-98F7B2B51D2D}" name="Previsão"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9C43B5B8-68DF-49B9-AD65-7073C784E948}" name="Tabela2" displayName="Tabela2" ref="A1:E6" totalsRowShown="0">
+  <tableColumns count="5">
+    <tableColumn id="5" xr3:uid="{78FAEF6E-9D28-4D09-BCBD-2A413A5F830F}" name="ID"/>
+    <tableColumn id="1" xr3:uid="{3FCA1E5E-E1A1-4F45-8BF4-5795A6091544}" name="Requisitos"/>
+    <tableColumn id="2" xr3:uid="{F85DC4DB-5B4F-4C29-A2D5-6408DF234282}" name="Classificação"/>
+    <tableColumn id="3" xr3:uid="{CE935F4E-7BC9-43DA-A5FD-4F734156506A}" name="Tamanho"/>
+    <tableColumn id="4" xr3:uid="{74D3FF3F-D87E-4ABB-B428-700F42A524F8}" name="Ordem Execução"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -459,22 +514,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2AFCCC-B644-4161-BC60-A749045AE6F7}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,92 +547,258 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>44322</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" t="str">
-        <f>IF(Tabela1[[#This Row],[Término]]=0, "Não finalizado",(Tabela1[[#This Row],[Início]]-Tabela1[[#This Row],[Término]]))</f>
-        <v>Não finalizado</v>
+      <c r="C2" s="1">
+        <v>44351</v>
+      </c>
+      <c r="D2">
+        <f>Tabela1[[#This Row],[Término]]-Tabela1[[#This Row],[Início]]</f>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44347</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44347</v>
+      </c>
+      <c r="D3">
+        <f>Tabela1[[#This Row],[Término]]-Tabela1[[#This Row],[Início]]</f>
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44347</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44350</v>
+      </c>
+      <c r="D4">
+        <f>Tabela1[[#This Row],[Término]]-Tabela1[[#This Row],[Início]]</f>
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44347</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44350</v>
+      </c>
+      <c r="D5" s="2">
+        <f>Tabela1[[#This Row],[Término]]-Tabela1[[#This Row],[Início]]</f>
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44353</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44353</v>
+      </c>
+      <c r="D6" s="2">
+        <f>Tabela1[[#This Row],[Término]]-Tabela1[[#This Row],[Início]]</f>
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44353</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44353</v>
+      </c>
+      <c r="D7" s="2">
+        <f>Tabela1[[#This Row],[Término]]-Tabela1[[#This Row],[Início]]</f>
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F225A6-6CD9-4D70-A3A7-B1FCA9B55781}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
         <v>13</v>
       </c>
-      <c r="G2" s="1">
-        <v>44346</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" t="str">
-        <f>IF(Tabela1[[#This Row],[Término]]=0, "Não finalizado",(Tabela1[[#This Row],[Início]]-Tabela1[[#This Row],[Término]]))</f>
-        <v>Não finalizado</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1">
-        <v>44331</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2" t="str">
-        <f>IF(Tabela1[[#This Row],[Término]]=0, "Não finalizado",(Tabela1[[#This Row],[Início]]-Tabela1[[#This Row],[Término]]))</f>
-        <v>Não finalizado</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="1">
-        <v>44336</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="2" t="str">
-        <f>IF(Tabela1[[#This Row],[Término]]=0, "Não finalizado",(Tabela1[[#This Row],[Início]]-Tabela1[[#This Row],[Término]]))</f>
-        <v>Não finalizado</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="1">
-        <v>44326</v>
+      <c r="E6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>